<commit_message>
Added 6 more students
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beecrowd\URI_Judge_Ranklist-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beecrowd\URI_Judge_Ranklist-master\URI-Leaderboard-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B803673E-0D2A-429D-A030-8C8DF8928B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8988078C-7510-40A1-91CF-301143177D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="231">
   <si>
     <t>Timestamp</t>
   </si>
@@ -659,6 +659,60 @@
   </si>
   <si>
     <t>https://www.beecrowd.com.br/judge/en/profile/613539</t>
+  </si>
+  <si>
+    <t>Mannat Mahajan</t>
+  </si>
+  <si>
+    <t>b21201</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/612381</t>
+  </si>
+  <si>
+    <t>Shambhabi Dhar</t>
+  </si>
+  <si>
+    <t>B21022</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/612401</t>
+  </si>
+  <si>
+    <t>Neha N</t>
+  </si>
+  <si>
+    <t>B21109</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613556</t>
+  </si>
+  <si>
+    <t>Saksham Panpaliya</t>
+  </si>
+  <si>
+    <t>B21126</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613558</t>
+  </si>
+  <si>
+    <t>Somesh</t>
+  </si>
+  <si>
+    <t>B21226</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613563</t>
+  </si>
+  <si>
+    <t>Rohan Chaudhary</t>
+  </si>
+  <si>
+    <t>B21119</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613561</t>
   </si>
 </sst>
 </file>
@@ -666,9 +720,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,6 +735,26 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -690,7 +764,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -713,18 +787,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1025,9 +1125,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2259,7 +2361,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>44570.970791331019</v>
       </c>
@@ -2275,11 +2377,141 @@
       <c r="E62" t="s">
         <v>88</v>
       </c>
-      <c r="F62" t="s">
-        <v>14</v>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>44571.028020833335</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>44571.046215277776</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>44571.049398148149</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>44571.060937499999</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
+        <v>44571.063356481478</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3">
+        <v>44571.06585648148</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D63" r:id="rId1" xr:uid="{B2E12FC7-413A-4975-B6A1-617EA82DCEF2}"/>
+    <hyperlink ref="D64" r:id="rId2" xr:uid="{A673BFF5-0729-4382-B45A-AB56B4FA5726}"/>
+    <hyperlink ref="D65" r:id="rId3" xr:uid="{E7819534-BC85-409E-BE0E-D3D697025D6D}"/>
+    <hyperlink ref="D66" r:id="rId4" xr:uid="{EA5025E8-2909-47B7-AA60-9CFB1DB4DBC8}"/>
+    <hyperlink ref="D67" r:id="rId5" xr:uid="{C418F52D-B815-4340-B57E-6B96B8A200F4}"/>
+    <hyperlink ref="D68" r:id="rId6" xr:uid="{C5ED3D60-5FDC-4D3A-A1D7-42C011B7240A}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more and fixed abhay pratap
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\beecrowd\URI_Judge_Ranklist-master\URI-Leaderboard-2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8D2A10-0E5B-4B3A-A8EB-916D619C374C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F4ECD8-99D3-47B3-B067-1BD93EA6E7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="282">
   <si>
     <t>Timestamp</t>
   </si>
@@ -340,9 +340,6 @@
     <t>B21029</t>
   </si>
   <si>
-    <t>https://www.beecrowd.com.br/judge/en/profile/612335</t>
-  </si>
-  <si>
     <t>CE</t>
   </si>
   <si>
@@ -821,6 +818,54 @@
   </si>
   <si>
     <t>https://www.beecrowd.com.br/judge/en/profile/612065</t>
+  </si>
+  <si>
+    <t>Rishiteja Reddy Narayan</t>
+  </si>
+  <si>
+    <t>B21306</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613963</t>
+  </si>
+  <si>
+    <t>Mantavya Gupta</t>
+  </si>
+  <si>
+    <t>B21015</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613295</t>
+  </si>
+  <si>
+    <t>Keshav verma</t>
+  </si>
+  <si>
+    <t>B21299</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/613531</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/614023</t>
+  </si>
+  <si>
+    <t>Pankaj</t>
+  </si>
+  <si>
+    <t>b21111</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/614024</t>
+  </si>
+  <si>
+    <t>Srijan</t>
+  </si>
+  <si>
+    <t>B21227</t>
+  </si>
+  <si>
+    <t>https://www.beecrowd.com.br/judge/en/profile/614021</t>
   </si>
 </sst>
 </file>
@@ -830,7 +875,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,13 +908,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Ubuntu"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -926,7 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -946,6 +1002,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1250,13 +1309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:F80"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.21875" customWidth="1"/>
@@ -1266,7 +1325,7 @@
     <col min="6" max="6" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>44569.711723900473</v>
       </c>
@@ -1306,7 +1365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>44569.715334687498</v>
       </c>
@@ -1326,7 +1385,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>44569.716415486109</v>
       </c>
@@ -1346,7 +1405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>44569.716672974537</v>
       </c>
@@ -1366,7 +1425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>44569.732542083337</v>
       </c>
@@ -1386,7 +1445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>44569.73954678241</v>
       </c>
@@ -1406,7 +1465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>44569.7400715162</v>
       </c>
@@ -1426,7 +1485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>44569.744375196758</v>
       </c>
@@ -1446,7 +1505,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>44569.749669953701</v>
       </c>
@@ -1466,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>44569.759106574071</v>
       </c>
@@ -1486,7 +1545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>44569.762565949073</v>
       </c>
@@ -1506,7 +1565,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>44569.781627025463</v>
       </c>
@@ -1526,7 +1585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>44569.7943452662</v>
       </c>
@@ -1546,7 +1605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>44569.794491666667</v>
       </c>
@@ -1566,7 +1625,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>44569.82203502315</v>
       </c>
@@ -1586,7 +1645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
         <v>44569.822576597217</v>
       </c>
@@ -1606,7 +1665,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>44569.826303796297</v>
       </c>
@@ -1626,7 +1685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
         <v>44569.849085462964</v>
       </c>
@@ -1646,7 +1705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
         <v>44569.870378819447</v>
       </c>
@@ -1666,7 +1725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
         <v>44569.871012152777</v>
       </c>
@@ -1686,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
         <v>44569.88371952546</v>
       </c>
@@ -1706,7 +1765,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
         <v>44569.905078854157</v>
       </c>
@@ -1726,7 +1785,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
         <v>44569.905535127313</v>
       </c>
@@ -1746,7 +1805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
         <v>44569.932461458331</v>
       </c>
@@ -1766,7 +1825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
         <v>44570.035225462962</v>
       </c>
@@ -1786,7 +1845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
         <v>44570.370627071759</v>
       </c>
@@ -1806,758 +1865,758 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>44570.396105868058</v>
+        <v>44570.40317730324</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2">
+        <v>44570.422817997693</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2">
+        <v>44570.429821886573</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2">
+        <v>44570.440302488423</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2">
+        <v>44570.460456134257</v>
+      </c>
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2">
+        <v>44570.479337627323</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2">
+        <v>44570.488596157411</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2">
+        <v>44570.548089826392</v>
+      </c>
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2">
+        <v>44570.550031099527</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2">
+        <v>44570.551580277781</v>
+      </c>
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="2">
+        <v>44570.556240104168</v>
+      </c>
+      <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="2">
+        <v>44570.565539629628</v>
+      </c>
+      <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="2">
+        <v>44570.576899583342</v>
+      </c>
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="2">
+        <v>44570.612495775473</v>
+      </c>
+      <c r="B41" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="2">
+        <v>44570.666036516202</v>
+      </c>
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2">
+        <v>44570.68315300926</v>
+      </c>
+      <c r="B43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2">
+        <v>44570.68163684028</v>
+      </c>
+      <c r="B44" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" t="s">
         <v>106</v>
       </c>
-      <c r="E28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>44570.40317730324</v>
-      </c>
-      <c r="B29" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" t="s">
-        <v>110</v>
-      </c>
-      <c r="E29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>44570.422817997693</v>
-      </c>
-      <c r="B30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>44570.429821886573</v>
-      </c>
-      <c r="B31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="2">
+        <v>44570.696259548611</v>
+      </c>
+      <c r="B45" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="2">
+        <v>44570.703678252306</v>
+      </c>
+      <c r="B46" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" t="s">
+        <v>164</v>
+      </c>
+      <c r="D46" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" t="s">
+        <v>96</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2">
+        <v>44570.705112199073</v>
+      </c>
+      <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="2">
+        <v>44570.705862268522</v>
+      </c>
+      <c r="B48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="2">
+        <v>44570.708216608793</v>
+      </c>
+      <c r="B49" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" t="s">
         <v>33</v>
       </c>
-      <c r="F31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>44570.440302488423</v>
-      </c>
-      <c r="B32" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="2">
+        <v>44570.747077893517</v>
+      </c>
+      <c r="B50" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" t="s">
+        <v>177</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="2">
+        <v>44570.772724166673</v>
+      </c>
+      <c r="B51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" t="s">
+        <v>180</v>
+      </c>
+      <c r="E51" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="2">
+        <v>44570.796978854167</v>
+      </c>
+      <c r="B52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" t="s">
+        <v>182</v>
+      </c>
+      <c r="D52" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="2">
+        <v>44570.80871005787</v>
+      </c>
+      <c r="B53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="2">
+        <v>44570.830188900472</v>
+      </c>
+      <c r="B54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="s">
+        <v>188</v>
+      </c>
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="2">
+        <v>44570.839812233797</v>
+      </c>
+      <c r="B55" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" t="s">
+        <v>191</v>
+      </c>
+      <c r="D55" t="s">
+        <v>192</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="2">
+        <v>44570.869622361111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>193</v>
+      </c>
+      <c r="C56" t="s">
+        <v>194</v>
+      </c>
+      <c r="D56" t="s">
+        <v>195</v>
+      </c>
+      <c r="E56" t="s">
+        <v>106</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="2">
+        <v>44570.88099597222</v>
+      </c>
+      <c r="B57" t="s">
+        <v>196</v>
+      </c>
+      <c r="C57" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" t="s">
+        <v>198</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="2">
+        <v>44570.920658923613</v>
+      </c>
+      <c r="B58" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E58" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="2">
+        <v>44570.956845462963</v>
+      </c>
+      <c r="B59" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" t="s">
+        <v>203</v>
+      </c>
+      <c r="D59" t="s">
+        <v>204</v>
+      </c>
+      <c r="E59" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="2">
+        <v>44570.960317129633</v>
+      </c>
+      <c r="B60" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" t="s">
+        <v>206</v>
+      </c>
+      <c r="D60" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" thickBot="1">
+      <c r="A61" s="2">
+        <v>44570.970791331019</v>
+      </c>
+      <c r="B61" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" t="s">
+        <v>210</v>
+      </c>
+      <c r="D61" t="s">
+        <v>211</v>
+      </c>
+      <c r="E61" t="s">
         <v>88</v>
       </c>
-      <c r="F32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>44570.460456134257</v>
-      </c>
-      <c r="B33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A62" s="3">
+        <v>44571.028020833335</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="F33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>44570.479337627323</v>
-      </c>
-      <c r="B34" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" t="s">
-        <v>126</v>
-      </c>
-      <c r="E34" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>44570.488596157411</v>
-      </c>
-      <c r="B35" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>44570.548089826392</v>
-      </c>
-      <c r="B36" t="s">
-        <v>131</v>
-      </c>
-      <c r="C36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>44570.550031099527</v>
-      </c>
-      <c r="B37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C37" t="s">
-        <v>135</v>
-      </c>
-      <c r="D37" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>44570.551580277781</v>
-      </c>
-      <c r="B38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" t="s">
-        <v>139</v>
-      </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>44570.556240104168</v>
-      </c>
-      <c r="B39" t="s">
-        <v>140</v>
-      </c>
-      <c r="C39" t="s">
-        <v>141</v>
-      </c>
-      <c r="D39" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>44570.565539629628</v>
-      </c>
-      <c r="B40" t="s">
-        <v>143</v>
-      </c>
-      <c r="C40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D40" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>44570.576899583342</v>
-      </c>
-      <c r="B41" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" t="s">
-        <v>147</v>
-      </c>
-      <c r="D41" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <v>44570.612495775473</v>
-      </c>
-      <c r="B42" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>44570.666036516202</v>
-      </c>
-      <c r="B43" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" t="s">
-        <v>153</v>
-      </c>
-      <c r="D43" t="s">
-        <v>154</v>
-      </c>
-      <c r="E43" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>44570.68315300926</v>
-      </c>
-      <c r="B44" t="s">
-        <v>155</v>
-      </c>
-      <c r="C44" t="s">
-        <v>156</v>
-      </c>
-      <c r="D44" t="s">
-        <v>157</v>
-      </c>
-      <c r="E44" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>44570.68163684028</v>
-      </c>
-      <c r="B45" t="s">
-        <v>158</v>
-      </c>
-      <c r="C45" t="s">
-        <v>159</v>
-      </c>
-      <c r="D45" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" t="s">
-        <v>107</v>
-      </c>
-      <c r="F45" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>44570.696259548611</v>
-      </c>
-      <c r="B46" t="s">
-        <v>161</v>
-      </c>
-      <c r="C46" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" t="s">
-        <v>163</v>
-      </c>
-      <c r="E46" t="s">
-        <v>107</v>
-      </c>
-      <c r="F46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>44570.703678252306</v>
-      </c>
-      <c r="B47" t="s">
-        <v>164</v>
-      </c>
-      <c r="C47" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" t="s">
-        <v>166</v>
-      </c>
-      <c r="E47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>44570.705112199073</v>
-      </c>
-      <c r="B48" t="s">
-        <v>167</v>
-      </c>
-      <c r="C48" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" t="s">
-        <v>169</v>
-      </c>
-      <c r="E48" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>44570.705862268522</v>
-      </c>
-      <c r="B49" t="s">
-        <v>170</v>
-      </c>
-      <c r="C49" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" t="s">
-        <v>172</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>44570.708216608793</v>
-      </c>
-      <c r="B50" t="s">
-        <v>173</v>
-      </c>
-      <c r="C50" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" t="s">
-        <v>175</v>
-      </c>
-      <c r="E50" t="s">
-        <v>33</v>
-      </c>
-      <c r="F50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>44570.747077893517</v>
-      </c>
-      <c r="B51" t="s">
-        <v>176</v>
-      </c>
-      <c r="C51" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" t="s">
-        <v>178</v>
-      </c>
-      <c r="E51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>44570.772724166673</v>
-      </c>
-      <c r="B52" t="s">
-        <v>179</v>
-      </c>
-      <c r="C52" t="s">
-        <v>180</v>
-      </c>
-      <c r="D52" t="s">
-        <v>181</v>
-      </c>
-      <c r="E52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>44570.796978854167</v>
-      </c>
-      <c r="B53" t="s">
-        <v>182</v>
-      </c>
-      <c r="C53" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" t="s">
-        <v>184</v>
-      </c>
-      <c r="E53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>44570.80871005787</v>
-      </c>
-      <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" t="s">
-        <v>186</v>
-      </c>
-      <c r="D54" t="s">
-        <v>187</v>
-      </c>
-      <c r="E54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>44570.830188900472</v>
-      </c>
-      <c r="B55" t="s">
-        <v>188</v>
-      </c>
-      <c r="C55" t="s">
-        <v>189</v>
-      </c>
-      <c r="D55" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>44570.839812233797</v>
-      </c>
-      <c r="B56" t="s">
-        <v>191</v>
-      </c>
-      <c r="C56" t="s">
-        <v>192</v>
-      </c>
-      <c r="D56" t="s">
-        <v>193</v>
-      </c>
-      <c r="E56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>44570.869622361111</v>
-      </c>
-      <c r="B57" t="s">
-        <v>194</v>
-      </c>
-      <c r="C57" t="s">
-        <v>195</v>
-      </c>
-      <c r="D57" t="s">
-        <v>196</v>
-      </c>
-      <c r="E57" t="s">
-        <v>107</v>
-      </c>
-      <c r="F57" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>44570.88099597222</v>
-      </c>
-      <c r="B58" t="s">
-        <v>197</v>
-      </c>
-      <c r="C58" t="s">
-        <v>198</v>
-      </c>
-      <c r="D58" t="s">
-        <v>199</v>
-      </c>
-      <c r="E58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>44570.920658923613</v>
-      </c>
-      <c r="B59" t="s">
-        <v>200</v>
-      </c>
-      <c r="C59" t="s">
-        <v>201</v>
-      </c>
-      <c r="D59" t="s">
-        <v>202</v>
-      </c>
-      <c r="E59" t="s">
-        <v>33</v>
-      </c>
-      <c r="F59" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>44570.956845462963</v>
-      </c>
-      <c r="B60" t="s">
-        <v>203</v>
-      </c>
-      <c r="C60" t="s">
-        <v>204</v>
-      </c>
-      <c r="D60" t="s">
-        <v>205</v>
-      </c>
-      <c r="E60" t="s">
-        <v>64</v>
-      </c>
-      <c r="F60" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>44570.960317129633</v>
-      </c>
-      <c r="B61" t="s">
-        <v>206</v>
-      </c>
-      <c r="C61" t="s">
-        <v>207</v>
-      </c>
-      <c r="D61" t="s">
-        <v>208</v>
-      </c>
-      <c r="E61" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
-        <v>44570.970791331019</v>
-      </c>
-      <c r="B62" t="s">
-        <v>210</v>
-      </c>
-      <c r="C62" t="s">
-        <v>211</v>
-      </c>
-      <c r="D62" t="s">
-        <v>212</v>
-      </c>
-      <c r="E62" t="s">
-        <v>88</v>
       </c>
       <c r="F62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="29.4" thickBot="1">
       <c r="A63" s="3">
-        <v>44571.028020833335</v>
+        <v>44571.046215277776</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="29.4" thickBot="1">
       <c r="A64" s="3">
-        <v>44571.046215277776</v>
+        <v>44571.049398148149</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="29.4" thickBot="1">
       <c r="A65" s="3">
-        <v>44571.049398148149</v>
+        <v>44571.060937499999</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
@@ -2566,138 +2625,138 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="29.4" thickBot="1">
       <c r="A66" s="3">
-        <v>44571.060937499999</v>
+        <v>44571.063356481478</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="29.4" thickBot="1">
       <c r="A67" s="3">
-        <v>44571.063356481478</v>
+        <v>44571.06585648148</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="29.4" thickBot="1">
       <c r="A68" s="3">
-        <v>44571.06585648148</v>
+        <v>44571.075416666667</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68">
+        <v>33</v>
+      </c>
+      <c r="F68" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="29.4" thickBot="1">
       <c r="A69" s="3">
-        <v>44571.075416666667</v>
+        <v>44571.332951388889</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F69" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="29.4" thickBot="1">
       <c r="A70" s="3">
-        <v>44571.332951388889</v>
+        <v>44571.401030092595</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F70" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="29.4" thickBot="1">
       <c r="A71" s="3">
-        <v>44571.401030092595</v>
+        <v>44571.499247685184</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="F71" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="29.4" thickBot="1">
       <c r="A72" s="3">
-        <v>44571.499247685184</v>
+        <v>44571.714039351849</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>64</v>
@@ -2706,189 +2765,295 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="29.4" thickBot="1">
       <c r="A73" s="3">
-        <v>44571.714039351849</v>
+        <v>44571.695752314816</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F73" s="4">
+      <c r="F73" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="29.4" thickBot="1">
       <c r="A74" s="3">
-        <v>44571.695752314816</v>
+        <v>44571.860752314817</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="F74" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="29.4" thickBot="1">
       <c r="A75" s="3">
-        <v>44571.860752314817</v>
+        <v>44571.978784722225</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="F75" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="29.4" thickBot="1">
       <c r="A76" s="3">
-        <v>44571.978784722225</v>
+        <v>44572.023657407408</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="6">
+        <v>96</v>
+      </c>
+      <c r="F76" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" ht="29.4" thickBot="1">
       <c r="A77" s="3">
-        <v>44572.023657407408</v>
+        <v>44572.055706018517</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="F77" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" ht="29.4" thickBot="1">
       <c r="A78" s="3">
-        <v>44572.055706018517</v>
+        <v>44572.651354166665</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="F78" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="29.4" thickBot="1">
       <c r="A79" s="3">
-        <v>44572.651354166665</v>
+        <v>44572.919027777774</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F79" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" ht="29.4" thickBot="1">
       <c r="A80" s="3">
-        <v>44572.919027777774</v>
+        <v>44573.010578703703</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="F80" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A81" s="3">
+        <v>44573.191030092596</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A82" s="3">
+        <v>44573.469618055555</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F82" s="8">
+        <v>85.306399999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A83" s="3">
+        <v>44573.487245370372</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A84" s="3">
+        <v>44573.490925925929</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="8">
+        <v>23.371400000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A85" s="3">
+        <v>44573.50545138889</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F85" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D63" r:id="rId1" xr:uid="{B2E12FC7-413A-4975-B6A1-617EA82DCEF2}"/>
-    <hyperlink ref="D64" r:id="rId2" xr:uid="{A673BFF5-0729-4382-B45A-AB56B4FA5726}"/>
-    <hyperlink ref="D65" r:id="rId3" xr:uid="{E7819534-BC85-409E-BE0E-D3D697025D6D}"/>
-    <hyperlink ref="D66" r:id="rId4" xr:uid="{EA5025E8-2909-47B7-AA60-9CFB1DB4DBC8}"/>
-    <hyperlink ref="D67" r:id="rId5" xr:uid="{C418F52D-B815-4340-B57E-6B96B8A200F4}"/>
-    <hyperlink ref="D68" r:id="rId6" xr:uid="{C5ED3D60-5FDC-4D3A-A1D7-42C011B7240A}"/>
-    <hyperlink ref="D69" r:id="rId7" xr:uid="{A8DBFA39-A1B3-451E-9FA9-52ED8F5B7D5C}"/>
-    <hyperlink ref="D70" r:id="rId8" display="http://www.beecrowd.com.br/judge/en/profile/613604" xr:uid="{10B02B12-A085-4D85-81CB-23EA64585B72}"/>
-    <hyperlink ref="D71" r:id="rId9" xr:uid="{FF4D8E14-F3B2-4B65-B2B5-A45599958753}"/>
-    <hyperlink ref="D72" r:id="rId10" xr:uid="{E49815E2-980F-4BF0-AA5F-1148BF6E6F4C}"/>
-    <hyperlink ref="D73" r:id="rId11" xr:uid="{67C300EF-4C4C-4FB0-81C7-A7C418E05E41}"/>
-    <hyperlink ref="D74" r:id="rId12" xr:uid="{F46E63D0-8CE9-4860-9926-5A36FBC87986}"/>
-    <hyperlink ref="D75" r:id="rId13" xr:uid="{A43D7100-BA73-415B-B87C-7FC65544C688}"/>
-    <hyperlink ref="D76" r:id="rId14" xr:uid="{783E7B08-F714-454B-B757-32427662ECB5}"/>
-    <hyperlink ref="D77" r:id="rId15" xr:uid="{0E282668-B302-45BD-9F8B-5622845974C3}"/>
-    <hyperlink ref="D78" r:id="rId16" xr:uid="{F669DA26-526B-4560-A6F9-7E8D8D554EC3}"/>
-    <hyperlink ref="D79" r:id="rId17" xr:uid="{6D7159D3-4270-474E-9147-E2ED23A4F909}"/>
-    <hyperlink ref="D80" r:id="rId18" xr:uid="{EC2AD195-C7EB-43B5-8C13-B4ED8CC6C11B}"/>
+    <hyperlink ref="D62" r:id="rId1" xr:uid="{B2E12FC7-413A-4975-B6A1-617EA82DCEF2}"/>
+    <hyperlink ref="D63" r:id="rId2" xr:uid="{A673BFF5-0729-4382-B45A-AB56B4FA5726}"/>
+    <hyperlink ref="D64" r:id="rId3" xr:uid="{E7819534-BC85-409E-BE0E-D3D697025D6D}"/>
+    <hyperlink ref="D65" r:id="rId4" xr:uid="{EA5025E8-2909-47B7-AA60-9CFB1DB4DBC8}"/>
+    <hyperlink ref="D66" r:id="rId5" xr:uid="{C418F52D-B815-4340-B57E-6B96B8A200F4}"/>
+    <hyperlink ref="D67" r:id="rId6" xr:uid="{C5ED3D60-5FDC-4D3A-A1D7-42C011B7240A}"/>
+    <hyperlink ref="D68" r:id="rId7" xr:uid="{A8DBFA39-A1B3-451E-9FA9-52ED8F5B7D5C}"/>
+    <hyperlink ref="D69" r:id="rId8" display="http://www.beecrowd.com.br/judge/en/profile/613604" xr:uid="{10B02B12-A085-4D85-81CB-23EA64585B72}"/>
+    <hyperlink ref="D70" r:id="rId9" xr:uid="{FF4D8E14-F3B2-4B65-B2B5-A45599958753}"/>
+    <hyperlink ref="D71" r:id="rId10" xr:uid="{E49815E2-980F-4BF0-AA5F-1148BF6E6F4C}"/>
+    <hyperlink ref="D72" r:id="rId11" xr:uid="{67C300EF-4C4C-4FB0-81C7-A7C418E05E41}"/>
+    <hyperlink ref="D73" r:id="rId12" xr:uid="{F46E63D0-8CE9-4860-9926-5A36FBC87986}"/>
+    <hyperlink ref="D74" r:id="rId13" xr:uid="{A43D7100-BA73-415B-B87C-7FC65544C688}"/>
+    <hyperlink ref="D75" r:id="rId14" xr:uid="{783E7B08-F714-454B-B757-32427662ECB5}"/>
+    <hyperlink ref="D76" r:id="rId15" xr:uid="{0E282668-B302-45BD-9F8B-5622845974C3}"/>
+    <hyperlink ref="D77" r:id="rId16" xr:uid="{F669DA26-526B-4560-A6F9-7E8D8D554EC3}"/>
+    <hyperlink ref="D78" r:id="rId17" xr:uid="{6D7159D3-4270-474E-9147-E2ED23A4F909}"/>
+    <hyperlink ref="D79" r:id="rId18" xr:uid="{EC2AD195-C7EB-43B5-8C13-B4ED8CC6C11B}"/>
+    <hyperlink ref="D80" r:id="rId19" xr:uid="{B6D94BDB-FA9B-42A0-8800-D9B2D1B96038}"/>
+    <hyperlink ref="D81" r:id="rId20" xr:uid="{DB239F54-5E99-47B0-9347-79D71B095E56}"/>
+    <hyperlink ref="D82" r:id="rId21" xr:uid="{0FC4D7A0-5F28-4027-8B78-77A8ACC00465}"/>
+    <hyperlink ref="D83" r:id="rId22" xr:uid="{C453CEE2-8119-4EDF-A5BA-BCCA0A7AFA29}"/>
+    <hyperlink ref="D84" r:id="rId23" xr:uid="{773954A5-0A12-4525-9A48-FDC5443A33B7}"/>
+    <hyperlink ref="D85" r:id="rId24" xr:uid="{7BEA6D2D-5E6C-4D77-BBEE-B9ECE4CFB2B7}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>